<commit_message>
Change to accounting for substitutions
</commit_message>
<xml_diff>
--- a/Data/Figure3/Figure3.xlsx
+++ b/Data/Figure3/Figure3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher.illingworth/Documents/Projects/MPhil_WithinHost/Writeup/Data/Figure3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopher.illingworth/Documents/GitHub/IVY/Data/Figure3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49686E2F-54F8-1A40-9E5C-7F357E8FA88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B44858B-3300-B343-82D0-51E025FC5F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8280" yWindow="5200" windowWidth="22420" windowHeight="15200" activeTab="1" xr2:uid="{96BCCD9A-C9B3-0E43-B7B2-68D0C77CF8E8}"/>
+    <workbookView xWindow="4300" yWindow="1840" windowWidth="22420" windowHeight="15200" activeTab="1" xr2:uid="{96BCCD9A-C9B3-0E43-B7B2-68D0C77CF8E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure3A" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
         <v>2</v>
       </c>
       <c r="C4">
-        <v>6.44876</v>
+        <v>6.86754</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -606,13 +606,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3.6882600000000001</v>
+        <v>3.2446299999999999</v>
       </c>
       <c r="D5">
-        <v>39.420699999999997</v>
+        <v>32.6248</v>
       </c>
       <c r="E5" s="2">
-        <v>11.0685</v>
+        <v>9.7372200000000007</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -625,7 +625,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>0.59908099999999997</v>
+        <v>6.86754</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -639,10 +639,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>14.953900000000001</v>
+        <v>14.2118</v>
       </c>
       <c r="D7">
-        <v>13.291600000000001</v>
+        <v>15.845700000000001</v>
       </c>
       <c r="E7" s="2"/>
       <c r="G7" s="2"/>
@@ -653,10 +653,10 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>25.551100000000002</v>
+        <v>27.209099999999999</v>
       </c>
       <c r="D8">
-        <v>45.427799999999998</v>
+        <v>45.511299999999999</v>
       </c>
       <c r="E8" s="2">
         <v>0</v>
@@ -672,16 +672,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>23.594799999999999</v>
+        <v>23.895199999999999</v>
       </c>
       <c r="D9">
-        <v>9.9291900000000002</v>
+        <v>28.180099999999999</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>34.3658</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2"/>
       <c r="I9" s="2"/>
@@ -691,22 +691,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="2">
-        <v>15.360300000000001</v>
+        <v>11.1753</v>
       </c>
       <c r="D10">
-        <v>22.929500000000001</v>
+        <v>11.485799999999999</v>
       </c>
       <c r="E10">
-        <v>10.4941</v>
+        <v>16.357299999999999</v>
       </c>
       <c r="F10">
-        <v>11.4648</v>
+        <v>22.971699999999998</v>
       </c>
       <c r="G10" s="2">
-        <v>8.8819199999999991</v>
+        <v>9.4584299999999999</v>
       </c>
       <c r="H10">
-        <v>17.197199999999999</v>
+        <v>17.2288</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -715,7 +715,7 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>2.2004299999999999</v>
+        <v>1.2848200000000001</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -731,7 +731,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC0E37-8827-2643-BD0F-12FFDBB62381}">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C9"/>
@@ -743,7 +743,7 @@
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
@@ -751,104 +751,60 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>11.531499999999999</v>
+        <v>10.0063</v>
       </c>
       <c r="C3">
-        <v>3.6882600000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+        <v>3.2446299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>14.589</v>
+        <v>14.5878</v>
       </c>
       <c r="C4">
-        <v>14.953900000000001</v>
-      </c>
-      <c r="G4">
-        <v>11.531499999999999</v>
-      </c>
-      <c r="H4">
-        <v>3.6882600000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+        <v>14.2118</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>29.914000000000001</v>
+        <v>31.421299999999999</v>
       </c>
       <c r="C5">
-        <v>25.551100000000002</v>
-      </c>
-      <c r="G5">
-        <v>14.589</v>
-      </c>
-      <c r="H5">
-        <v>14.953900000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+        <v>27.209099999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>20.595199999999998</v>
+        <v>24.881399999999999</v>
       </c>
       <c r="C6">
-        <v>23.594799999999999</v>
-      </c>
-      <c r="G6">
-        <v>29.914000000000001</v>
-      </c>
-      <c r="H6">
-        <v>25.551100000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+        <v>23.895199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>17.021699999999999</v>
+        <v>11.2468</v>
       </c>
       <c r="C7">
-        <v>15.360300000000001</v>
-      </c>
-      <c r="G7">
-        <v>20.595199999999998</v>
-      </c>
-      <c r="H7">
-        <v>23.594799999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+        <v>11.1753</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>10.7072</v>
+        <v>17.8796</v>
       </c>
       <c r="C8">
-        <v>10.4941</v>
-      </c>
-      <c r="G8">
-        <v>17.021699999999999</v>
-      </c>
-      <c r="H8">
-        <v>15.360300000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+        <v>16.357299999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>10.707100000000001</v>
+        <v>11.246700000000001</v>
       </c>
       <c r="C9">
-        <v>8.8819199999999991</v>
-      </c>
-      <c r="G9">
-        <v>10.7072</v>
-      </c>
-      <c r="H9">
-        <v>10.4941</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="G10">
-        <v>10.707100000000001</v>
-      </c>
-      <c r="H10">
-        <v>8.8819199999999991</v>
+        <v>9.4584299999999999</v>
       </c>
     </row>
   </sheetData>
@@ -858,7 +814,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9BD789F-6604-D14F-BD3A-086F37AE2A9A}">
-  <dimension ref="B2:I10"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:C9"/>
@@ -869,7 +825,7 @@
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -877,104 +833,60 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>11.531499999999999</v>
+        <v>10.0063</v>
       </c>
       <c r="C3">
-        <v>9.3561400000000003E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+        <v>9.9452899999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>14.589</v>
+        <v>14.5878</v>
       </c>
       <c r="C4">
-        <v>1.1250599999999999</v>
-      </c>
-      <c r="H4">
-        <v>11.531499999999999</v>
-      </c>
-      <c r="I4">
-        <v>9.3561400000000003E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.89688800000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>29.914000000000001</v>
+        <v>31.421299999999999</v>
       </c>
       <c r="C5">
-        <v>0.56245599999999996</v>
-      </c>
-      <c r="H5">
-        <v>14.589</v>
-      </c>
-      <c r="I5">
-        <v>1.1250599999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.597854</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>20.595199999999998</v>
+        <v>24.881399999999999</v>
       </c>
       <c r="C6">
-        <v>2.3763100000000001</v>
-      </c>
-      <c r="H6">
-        <v>29.914000000000001</v>
-      </c>
-      <c r="I6">
-        <v>0.56245599999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.84794700000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>17.021699999999999</v>
+        <v>11.2468</v>
       </c>
       <c r="C7">
-        <v>0.66988999999999999</v>
-      </c>
-      <c r="H7">
-        <v>20.595199999999998</v>
-      </c>
-      <c r="I7">
-        <v>2.3763100000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.97296099999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>10.7072</v>
+        <v>17.8796</v>
       </c>
       <c r="C8">
-        <v>0.91533799999999998</v>
-      </c>
-      <c r="H8">
-        <v>17.021699999999999</v>
-      </c>
-      <c r="I8">
-        <v>0.66988999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+        <v>0.71206199999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>10.707100000000001</v>
+        <v>11.246700000000001</v>
       </c>
       <c r="C9">
-        <v>0.51647600000000005</v>
-      </c>
-      <c r="H9">
-        <v>10.7072</v>
-      </c>
-      <c r="I9">
-        <v>0.91533799999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="H10">
-        <v>10.707100000000001</v>
-      </c>
-      <c r="I10">
-        <v>0.51647600000000005</v>
+        <v>0.54898999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>